<commit_message>
Suite class is added for serial execution.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Ashish_05</t>
-  </si>
-  <si>
-    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -411,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +419,7 @@
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -444,7 +441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -455,7 +452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -465,11 +462,8 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -480,7 +474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>

</xml_diff>